<commit_message>
PROS-10194 - CCRU - Promo tracking KPIs
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPI_Promo_Tracking.xlsx
+++ b/Projects/CCRU/Data/KPI_Promo_Tracking.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">PROMO_COMPLIANCE_PRICE_TARGET</t>
   </si>
   <si>
-    <t xml:space="preserve">Main Shelves</t>
+    <t xml:space="preserve">Main Shelf</t>
   </si>
 </sst>
 </file>
@@ -298,17 +298,17 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.6989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="61.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="57.7397959183674"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="11.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="65.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.3775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>